<commit_message>
Agregar actividades y calificaciones
</commit_message>
<xml_diff>
--- a/lms/moodle/endpoints.xlsx
+++ b/lms/moodle/endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\campusoft\git knowledge_base\knowledge_base\lms\moodle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EA7D60-B170-428E-9521-F321A5E2C7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4DD598-9284-4D92-BC1C-73027A85C1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" xr2:uid="{3CA9E647-28ED-4C45-972F-1B8A924355E7}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{3CA9E647-28ED-4C45-972F-1B8A924355E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="229">
   <si>
     <t>Entidad</t>
   </si>
@@ -369,9 +369,6 @@
   </si>
   <si>
     <t>Presenta error genérico si no existe el curso y expícito para rol y usuario</t>
-  </si>
-  <si>
-    <t>Presenta error si no existe el curso</t>
   </si>
   <si>
     <t>Presenta error de categoría desconocida</t>
@@ -3966,6 +3963,63 @@
   </si>
   <si>
     <t>Los campos especificados en la columna ¿Requiere entrada? Son los obligatorios, el resto de campos se puede consultar en la pestaña campos</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Grades</t>
+  </si>
+  <si>
+    <t>OBTENER GRADES POR CURSO</t>
+  </si>
+  <si>
+    <t>Permite obtener calificaciones de un curso</t>
+  </si>
+  <si>
+    <t>OBTENER GRADES POR USUARIO</t>
+  </si>
+  <si>
+    <t>Permite obtener calificaciones finales por usuario</t>
+  </si>
+  <si>
+    <t>gradereport_user_get_grade_items</t>
+  </si>
+  <si>
+    <t>gradereport_overview_get_course_grades</t>
+  </si>
+  <si>
+    <t>Objeto usergrades que contiene un array de grades</t>
+  </si>
+  <si>
+    <t>Presenta error específico de curso no existente</t>
+  </si>
+  <si>
+    <t>Presenta información de todos los estudiantes tengan o no calificaciones</t>
+  </si>
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>userid=int</t>
+  </si>
+  <si>
+    <t>Objeto grades que contiene un array de courseid, grade, rawgrade y un objeto warnings</t>
+  </si>
+  <si>
+    <t>Presenta error específico de user no existente</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>No existe un endpoint para listar las actividades pero se puede utilizar el endpoint gradereport_user_get_grade_items y filtrar los datos de las actividades</t>
+  </si>
+  <si>
+    <t>No existe un endpoint para listar los roles existentes</t>
+  </si>
+  <si>
+    <t>Presenta error específico de curso inválido</t>
   </si>
 </sst>
 </file>
@@ -4452,7 +4506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A88059-AE27-4B51-A9CA-14DCA16A9645}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4463,62 +4517,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="240" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -4529,11 +4583,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D16DB1-5039-47C1-A228-BB1620FB4ABB}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4703,7 +4757,7 @@
         <v>8</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>60</v>
@@ -4744,7 +4798,7 @@
         <v>55</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>61</v>
@@ -4785,7 +4839,7 @@
         <v>55</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>62</v>
@@ -4852,7 +4906,7 @@
         <v>71</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>6</v>
@@ -4899,7 +4953,7 @@
         <v>75</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>76</v>
@@ -4940,7 +4994,7 @@
         <v>82</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>79</v>
@@ -4981,7 +5035,7 @@
         <v>82</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>83</v>
@@ -5094,7 +5148,7 @@
         <v>11</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M14" s="8" t="s">
         <v>92</v>
@@ -5135,7 +5189,7 @@
         <v>55</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>94</v>
@@ -5176,7 +5230,7 @@
         <v>55</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>98</v>
@@ -5217,7 +5271,7 @@
         <v>100</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>106</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="135" x14ac:dyDescent="0.25">
@@ -5255,23 +5309,120 @@
         <v>105</v>
       </c>
       <c r="M18" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>118</v>
-      </c>
+      <c r="B21" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="M22" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M21" xr:uid="{E6D16DB1-5039-47C1-A228-BB1620FB4ABB}"/>
@@ -5312,400 +5463,400 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>